<commit_message>
Finish CLI testing routines.
</commit_message>
<xml_diff>
--- a/tests/data/surgeo_output.xlsx
+++ b/tests/data/surgeo_output.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theon\development\surgeo\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8711BDAC-45CE-4E90-A539-2E22D6011A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384593C2-5FE8-4362-B766-6F8BFFC91746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="370" windowWidth="19030" windowHeight="14070"/>
+    <workbookView xWindow="0" yWindow="370" windowWidth="19030" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="surgeo_output" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,8 +536,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -892,10 +893,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -926,7 +929,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>631</v>
       </c>
       <c r="B2" t="s">

</xml_diff>

<commit_message>
Use the "Other" entries for first_name and surname when names are not present
</commit_message>
<xml_diff>
--- a/tests/data/surgeo_output.xlsx
+++ b/tests/data/surgeo_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theon\development\surgeo\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam.weeden/Dev/surgeo/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384593C2-5FE8-4362-B766-6F8BFFC91746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10DE955-E83C-9C40-A187-9747AA7DA500}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="370" windowWidth="19030" windowHeight="14070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19040" windowHeight="14080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="surgeo_output" sheetId="1" r:id="rId1"/>
@@ -897,12 +897,12 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -928,7 +928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>631</v>
       </c>
@@ -954,12 +954,30 @@
         <v>0.97565537297756</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>63110</v>
       </c>
+      <c r="C3">
+        <v>0.58709999999999996</v>
+      </c>
+      <c r="D3">
+        <v>0.30370000000000003</v>
+      </c>
+      <c r="E3">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="F3">
+        <v>2.3E-3</v>
+      </c>
+      <c r="G3">
+        <v>3.15E-2</v>
+      </c>
+      <c r="H3">
+        <v>1.8700000000000001E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>

</xml_diff>